<commit_message>
new structure works and gives same output as old version
</commit_message>
<xml_diff>
--- a/output/ind_demand_projections_per_country.xlsx
+++ b/output/ind_demand_projections_per_country.xlsx
@@ -1516,13 +1516,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>4.799113573794</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>20.154261382235</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -1572,13 +1572,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.865289707205</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>3.633853348586</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -1628,13 +1628,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>15.391583202062</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>64.63818498371501</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -1712,13 +1712,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>4.898807391966</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>20.572933547154</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -1740,13 +1740,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>8.374068538641</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>35.167570753506</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -1796,13 +1796,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>4.16307879918</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>17.483182463462</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -1880,13 +1880,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>1.441627316874</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>6.054229247397</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1908,13 +1908,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>7.980467908803</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>33.514613420451</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1936,13 +1936,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>0.802656608897</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>3.37082064159</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1964,13 +1964,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>1.45206730024</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>6.098072792741</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -1992,13 +1992,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>0.570597942022</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>2.396271705357</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -2020,13 +2020,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>0.967559246887</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>4.063342462042</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -2076,13 +2076,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>0.135509342673</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>0.569082325303</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -2104,13 +2104,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>0.673124482688</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>2.826840115006</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -2132,13 +2132,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>1.077326254146</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>4.524317790385</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -2188,13 +2188,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>0.7041312999979999</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>2.957055724845</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -2328,13 +2328,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>0.407193093593</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>1.710039971991</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -2412,13 +2412,13 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>0.203651533969</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>0.855250909026</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -2529,13 +2529,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>6.183840146639</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>21.368267865987</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -2585,13 +2585,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>3.488426587297</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>12.054262720344</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -2641,13 +2641,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>26.377181363701</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>91.146385346918</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -2725,13 +2725,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>4.263557039335</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>14.732727030136</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -2753,13 +2753,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>8.318069019093</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>28.743098578376</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -2781,13 +2781,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>0.126050978656</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.435569324696</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -2809,13 +2809,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>7.393434190161</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>25.548021695026</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -2893,13 +2893,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>3.696888147066</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>12.774601917879</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -2921,13 +2921,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>18.300894570125</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>63.238765570966</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -2977,13 +2977,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>4.395378608096</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>15.188236636626</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -3005,13 +3005,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>2.390151897629</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>8.259173066868</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -3033,13 +3033,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>0.336608596245</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>1.163151452817</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -3089,13 +3089,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>0.967295360263</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>3.3424904062</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -3145,13 +3145,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>0.08182850811800001</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>0.28275851883</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -3173,13 +3173,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>0.524685748113</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>1.81305230169</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -3453,13 +3453,13 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0</v>
+        <v>2.3774111e-05</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>8.2151473e-05</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -10633,25 +10633,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.749303456238</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>3.54123126593</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.128204385307</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.119681803308</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>3.293345077315</v>
       </c>
     </row>
     <row r="3">
@@ -10661,25 +10661,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.066084056818</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.39932540022</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.01445691163</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.013495866386</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>0.371372622205</v>
       </c>
     </row>
     <row r="4">
@@ -10689,25 +10689,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.555366753202</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>2.450654169388</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.08872185626699999</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.08282393558999999</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>2.279108377531</v>
       </c>
     </row>
     <row r="5">
@@ -10717,25 +10717,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.23530089849</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.44448016057</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.01609166459</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.01502194665</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>0.41336654933</v>
       </c>
     </row>
     <row r="6">
@@ -10745,25 +10745,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>2.720832104454</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>12.006153595873</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.43466281247</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.405767939241</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>11.165722844162</v>
       </c>
     </row>
     <row r="7">
@@ -10773,25 +10773,25 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.019295664914</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.058133476763</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.002104625791</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.001964717582</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>0.054064133389</v>
       </c>
     </row>
     <row r="8">
@@ -10801,25 +10801,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.118656700372</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>0.506141815642</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.018324022206</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.017105904889</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>0.470711888547</v>
       </c>
     </row>
     <row r="9">
@@ -10829,25 +10829,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>1.226794085713</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>5.948002998634</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.215337550975</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.201022658929</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>5.531642788729</v>
       </c>
     </row>
     <row r="10">
@@ -10857,25 +10857,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>2.215788374186</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>10.347064358161</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.374598247375</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.349696257696</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>9.622769853089</v>
       </c>
     </row>
     <row r="11">
@@ -10885,25 +10885,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>0.272015517415</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.991550320494</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>0.035897429395</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.03351109304</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>0.92214179806</v>
       </c>
     </row>
     <row r="12">
@@ -10913,25 +10913,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>1.573553287855</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>8.362628150734</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.302755036625</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>0.282628933927</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>7.777244180183</v>
       </c>
     </row>
     <row r="13">
@@ -10941,25 +10941,25 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>0.0258106384</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>0.078685873341</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>0.00284869111</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>0.002659320024</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>0.073177862207</v>
       </c>
     </row>
     <row r="14">
@@ -10969,25 +10969,25 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>0.119992415542</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>0.52948778757</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>0.019169224271</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>0.017894920859</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>0.49242364244</v>
       </c>
     </row>
     <row r="15">
@@ -10997,25 +10997,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>0.323800601291</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1.195055536105</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>0.043264997089</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>0.040388890438</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>1.111401648578</v>
       </c>
     </row>
     <row r="16">
@@ -11025,25 +11025,25 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>0.508133437694</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>2.242228798377</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>0.08117616253399999</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>0.075779853353</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>2.085272782491</v>
       </c>
     </row>
     <row r="17">
@@ -11081,25 +11081,25 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>1.123147363811</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>4.143530397541</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>0.150009623129</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>0.140037504698</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>3.853483269713</v>
       </c>
     </row>
     <row r="19">
@@ -11109,25 +11109,25 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>0.442264570837</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>2.299942862277</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>0.08326560417999999</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>0.077730396179</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>2.138946861918</v>
       </c>
     </row>
     <row r="20">
@@ -11137,25 +11137,25 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>0.147649917102</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>0.898098865685</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>0.032514174979</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>0.030352745619</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>0.835231945087</v>
       </c>
     </row>
     <row r="21">
@@ -11165,25 +11165,25 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>0.107021745219</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>0.137199369971</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>0.004967074887</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>0.004636881011</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>0.127595414073</v>
       </c>
     </row>
     <row r="22">
@@ -11193,25 +11193,25 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>0.223982848528</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>0.666777129236</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>0.024139556434</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>0.022534842612</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>0.62010273019</v>
       </c>
     </row>
     <row r="23">
@@ -11221,25 +11221,25 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>0.362996286569</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1.032956792561</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>0.037396481815</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>0.034910493664</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>0.960649817082</v>
       </c>
     </row>
     <row r="24">
@@ -11249,25 +11249,25 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>0.238484915361</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>0.741060586684</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>0.026828865402</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>0.025045375666</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>0.689186345616</v>
       </c>
     </row>
     <row r="25">
@@ -11277,25 +11277,25 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>1.196792523611</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>5.633315769352</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>0.203944823485</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>0.19038728037</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>5.238983665497</v>
       </c>
     </row>
     <row r="26">
@@ -11445,25 +11445,25 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>0.032123126051</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>0.175122848469</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>0.006340031321</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>0.005918568072</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>0.162864249076</v>
       </c>
     </row>
     <row r="32">
@@ -11529,25 +11529,25 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>0.049111008522</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>0.060024565972</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>0.002173089529</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>0.002028630089</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>0.055822846354</v>
       </c>
     </row>
     <row r="35">
@@ -11557,25 +11557,25 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0</v>
+        <v>0.037273516304</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>0.20320078243</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>0.007356546198</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>0.006867508572</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>0.18897672766</v>
       </c>
     </row>
   </sheetData>
@@ -12659,25 +12659,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11.510019026232</v>
+        <v>35.339664990665</v>
       </c>
       <c r="C2" t="n">
-        <v>21.637766967882</v>
+        <v>25.178998233812</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>91.25258076503501</v>
       </c>
       <c r="E2" t="n">
-        <v>1.45613338415</v>
+        <v>1.584337769456</v>
       </c>
       <c r="F2" t="n">
-        <v>1.763799064942</v>
+        <v>1.883480868251</v>
       </c>
       <c r="G2" t="n">
         <v>6.170611856456</v>
       </c>
       <c r="H2" t="n">
-        <v>12.247222662333</v>
+        <v>15.540567739648</v>
       </c>
     </row>
     <row r="3">
@@ -12687,25 +12687,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.959239514038</v>
+        <v>3.587367952888</v>
       </c>
       <c r="C3" t="n">
-        <v>5.868193233169</v>
+        <v>6.300329327281</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1.916625881393</v>
       </c>
       <c r="E3" t="n">
-        <v>0.594032430461</v>
+        <v>0.6144286249649999</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5180227198289999</v>
+        <v>0.533453869875</v>
       </c>
       <c r="G3" t="n">
-        <v>1.505245457274</v>
+        <v>1.50655788503</v>
       </c>
       <c r="H3" t="n">
-        <v>3.250892625605</v>
+        <v>3.645888947412</v>
       </c>
     </row>
     <row r="4">
@@ -12715,25 +12715,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5.366378246682</v>
+        <v>11.490360050914</v>
       </c>
       <c r="C4" t="n">
-        <v>18.675214268628</v>
+        <v>21.163101726393</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>20.503099276167</v>
       </c>
       <c r="E4" t="n">
-        <v>1.241632492837</v>
+        <v>1.337094195348</v>
       </c>
       <c r="F4" t="n">
-        <v>1.686179763224</v>
+        <v>1.77119984178</v>
       </c>
       <c r="G4" t="n">
-        <v>6.026792258868</v>
+        <v>6.028281590403</v>
       </c>
       <c r="H4" t="n">
-        <v>9.720609753699</v>
+        <v>12.026526098861</v>
       </c>
     </row>
     <row r="5">
@@ -12743,25 +12743,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.775748674337</v>
+        <v>1.024277331248</v>
       </c>
       <c r="C5" t="n">
-        <v>2.282256916342</v>
+        <v>2.789080275285</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.002901343633</v>
       </c>
       <c r="E5" t="n">
-        <v>0.133214518079</v>
+        <v>0.160591341453</v>
       </c>
       <c r="F5" t="n">
-        <v>0.121926081486</v>
+        <v>0.140625236962</v>
       </c>
       <c r="G5" t="n">
-        <v>0.44454848999</v>
+        <v>0.447042217925</v>
       </c>
       <c r="H5" t="n">
-        <v>1.582567826786</v>
+        <v>2.040821478945</v>
       </c>
     </row>
     <row r="6">
@@ -12771,25 +12771,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>76.22941002054699</v>
+        <v>147.079561921193</v>
       </c>
       <c r="C6" t="n">
-        <v>128.317868952736</v>
+        <v>142.316530588875</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>261.482648963137</v>
       </c>
       <c r="E6" t="n">
-        <v>9.071762690019</v>
+        <v>9.867102692621</v>
       </c>
       <c r="F6" t="n">
-        <v>11.857023771322</v>
+        <v>12.380316450094</v>
       </c>
       <c r="G6" t="n">
-        <v>41.204945339455</v>
+        <v>41.284645661065</v>
       </c>
       <c r="H6" t="n">
-        <v>66.184137151941</v>
+        <v>78.784465785094</v>
       </c>
     </row>
     <row r="7">
@@ -12799,25 +12799,25 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.609838235682</v>
+        <v>0.6291339005960001</v>
       </c>
       <c r="C7" t="n">
-        <v>2.487344865091</v>
+        <v>2.545478341853</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.094155061239</v>
+        <v>0.09625968703</v>
       </c>
       <c r="F7" t="n">
-        <v>0.007183934048</v>
+        <v>0.009148651630000001</v>
       </c>
       <c r="G7" t="n">
         <v>0.104234061602</v>
       </c>
       <c r="H7" t="n">
-        <v>2.281771808202</v>
+        <v>2.335835941591</v>
       </c>
     </row>
     <row r="8">
@@ -12827,25 +12827,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5.902852798088</v>
+        <v>6.113168093161</v>
       </c>
       <c r="C8" t="n">
-        <v>12.618922579694</v>
+        <v>13.132489058536</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.311133572002</v>
       </c>
       <c r="E8" t="n">
-        <v>0.539241707482</v>
+        <v>0.558909717569</v>
       </c>
       <c r="F8" t="n">
-        <v>0.203801424117</v>
+        <v>0.221345260293</v>
       </c>
       <c r="G8" t="n">
-        <v>1.072939876694</v>
+        <v>1.073236863222</v>
       </c>
       <c r="H8" t="n">
-        <v>10.802939571401</v>
+        <v>11.278997217452</v>
       </c>
     </row>
     <row r="9">
@@ -12855,25 +12855,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>34.891791418535</v>
+        <v>49.305453647516</v>
       </c>
       <c r="C9" t="n">
-        <v>57.21539120993</v>
+        <v>63.772633648584</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>51.155460067742</v>
       </c>
       <c r="E9" t="n">
-        <v>3.299890387102</v>
+        <v>3.625510438777</v>
       </c>
       <c r="F9" t="n">
-        <v>2.932869908551</v>
+        <v>3.169827532386</v>
       </c>
       <c r="G9" t="n">
-        <v>10.947819472909</v>
+        <v>10.97218905051</v>
       </c>
       <c r="H9" t="n">
-        <v>40.034811441368</v>
+        <v>46.005106626912</v>
       </c>
     </row>
     <row r="10">
@@ -12883,25 +12883,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>33.072599593757</v>
+        <v>63.494146008399</v>
       </c>
       <c r="C10" t="n">
-        <v>40.668136233618</v>
+        <v>51.548296048863</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>110.843643038932</v>
       </c>
       <c r="E10" t="n">
-        <v>3.310701889603</v>
+        <v>3.781799306691</v>
       </c>
       <c r="F10" t="n">
-        <v>4.31382649915</v>
+        <v>4.694966496833</v>
       </c>
       <c r="G10" t="n">
-        <v>14.171421606576</v>
+        <v>14.19274542486</v>
       </c>
       <c r="H10" t="n">
-        <v>18.872186238289</v>
+        <v>28.878784820479</v>
       </c>
     </row>
     <row r="11">
@@ -12911,25 +12911,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.259355732496</v>
+        <v>2.22577776807</v>
       </c>
       <c r="C11" t="n">
-        <v>3.126965746996</v>
+        <v>4.123583041177</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>2.393117889847</v>
       </c>
       <c r="E11" t="n">
-        <v>0.134821207542</v>
+        <v>0.171635843691</v>
       </c>
       <c r="F11" t="n">
-        <v>0.07514729861</v>
+        <v>0.10895725858</v>
       </c>
       <c r="G11" t="n">
-        <v>0.35762543328</v>
+        <v>0.357828112227</v>
       </c>
       <c r="H11" t="n">
-        <v>2.559371807565</v>
+        <v>3.485161826679</v>
       </c>
     </row>
     <row r="12">
@@ -12939,25 +12939,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>37.052229308196</v>
+        <v>54.995928838227</v>
       </c>
       <c r="C12" t="n">
-        <v>66.85524887732301</v>
+        <v>76.866180030408</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>61.473070552521</v>
       </c>
       <c r="E12" t="n">
-        <v>3.917924232647</v>
+        <v>4.519049606234</v>
       </c>
       <c r="F12" t="n">
-        <v>4.428536029523</v>
+        <v>4.808387347051</v>
       </c>
       <c r="G12" t="n">
-        <v>16.446049735165</v>
+        <v>16.511981855259</v>
       </c>
       <c r="H12" t="n">
-        <v>42.062738879989</v>
+        <v>51.026761221864</v>
       </c>
     </row>
     <row r="13">
@@ -12967,25 +12967,25 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.182987077404</v>
+        <v>0.208797715804</v>
       </c>
       <c r="C13" t="n">
-        <v>0.56076235355</v>
+        <v>0.63944822689</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0.019217264596</v>
+        <v>0.022065955706</v>
       </c>
       <c r="F13" t="n">
-        <v>0.001145768649</v>
+        <v>0.003805088674</v>
       </c>
       <c r="G13" t="n">
         <v>0.026787274619</v>
       </c>
       <c r="H13" t="n">
-        <v>0.513612045685</v>
+        <v>0.586789907892</v>
       </c>
     </row>
     <row r="14">
@@ -12995,25 +12995,25 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.395337213804</v>
+        <v>1.515329629346</v>
       </c>
       <c r="C14" t="n">
-        <v>1.645144919728</v>
+        <v>2.174632707298</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0.058041007203</v>
+        <v>0.077210231474</v>
       </c>
       <c r="F14" t="n">
-        <v>0.028671722424</v>
+        <v>0.046566643283</v>
       </c>
       <c r="G14" t="n">
         <v>0.176615257831</v>
       </c>
       <c r="H14" t="n">
-        <v>1.381816932269</v>
+        <v>1.874240574709</v>
       </c>
     </row>
     <row r="15">
@@ -13023,25 +13023,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2.400516007142</v>
+        <v>10.727699975373</v>
       </c>
       <c r="C15" t="n">
-        <v>4.63948908559</v>
+        <v>5.959518888881</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>30.368723434658</v>
       </c>
       <c r="E15" t="n">
-        <v>0.314510342142</v>
+        <v>0.380397766151</v>
       </c>
       <c r="F15" t="n">
-        <v>0.366996176429</v>
+        <v>0.414756464072</v>
       </c>
       <c r="G15" t="n">
-        <v>1.246921608125</v>
+        <v>1.251920578813</v>
       </c>
       <c r="H15" t="n">
-        <v>2.711060958893</v>
+        <v>3.912444079845</v>
       </c>
     </row>
     <row r="16">
@@ -13051,25 +13051,25 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>11.29318018344</v>
+        <v>51.988453176495</v>
       </c>
       <c r="C16" t="n">
-        <v>15.956712314503</v>
+        <v>18.261822924499</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>152.766053424734</v>
       </c>
       <c r="E16" t="n">
-        <v>1.096087372286</v>
+        <v>1.188646191585</v>
       </c>
       <c r="F16" t="n">
-        <v>1.498953013186</v>
+        <v>1.578441844562</v>
       </c>
       <c r="G16" t="n">
-        <v>5.266889037695</v>
+        <v>5.26940431016</v>
       </c>
       <c r="H16" t="n">
-        <v>8.094782891335001</v>
+        <v>10.225330578192</v>
       </c>
     </row>
     <row r="17">
@@ -13079,25 +13079,25 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>8.854433788890001</v>
+        <v>11.224102343078</v>
       </c>
       <c r="C17" t="n">
-        <v>27.128424886536</v>
+        <v>27.504200452498</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>9.119645263137</v>
       </c>
       <c r="E17" t="n">
-        <v>2.647654254658</v>
+        <v>2.715675899998</v>
       </c>
       <c r="F17" t="n">
-        <v>3.864584320626</v>
+        <v>3.886748811117</v>
       </c>
       <c r="G17" t="n">
-        <v>12.39868263171</v>
+        <v>12.413713654349</v>
       </c>
       <c r="H17" t="n">
-        <v>8.217503679541</v>
+        <v>8.488062087035001</v>
       </c>
     </row>
     <row r="18">
@@ -13107,25 +13107,25 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>12.596308710147</v>
+        <v>25.014899942076</v>
       </c>
       <c r="C18" t="n">
-        <v>30.167825571421</v>
+        <v>34.359537349489</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>41.474630778511</v>
       </c>
       <c r="E18" t="n">
-        <v>2.066196916795</v>
+        <v>2.22492817346</v>
       </c>
       <c r="F18" t="n">
-        <v>1.9245219104</v>
+        <v>2.067401312888</v>
       </c>
       <c r="G18" t="n">
-        <v>6.700073510896</v>
+        <v>6.702000766117</v>
       </c>
       <c r="H18" t="n">
-        <v>19.47703323333</v>
+        <v>23.365207097023</v>
       </c>
     </row>
     <row r="19">
@@ -13135,25 +13135,25 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>5.507950699488</v>
+        <v>10.109951480753</v>
       </c>
       <c r="C19" t="n">
-        <v>17.364536461173</v>
+        <v>19.709474111143</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>15.652892113115</v>
       </c>
       <c r="E19" t="n">
-        <v>1.615540970966</v>
+        <v>1.706951382227</v>
       </c>
       <c r="F19" t="n">
-        <v>2.156763127351</v>
+        <v>2.237147465496</v>
       </c>
       <c r="G19" t="n">
-        <v>6.825212810757</v>
+        <v>6.827012602265</v>
       </c>
       <c r="H19" t="n">
-        <v>6.767019552099</v>
+        <v>8.938362661155001</v>
       </c>
     </row>
     <row r="20">
@@ -13163,25 +13163,25 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>11.302925027867</v>
+        <v>14.056481191441</v>
       </c>
       <c r="C20" t="n">
-        <v>18.5382714591</v>
+        <v>19.4639775502</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>9.698948804879</v>
       </c>
       <c r="E20" t="n">
-        <v>0.703986409989</v>
+        <v>0.7414979532530001</v>
       </c>
       <c r="F20" t="n">
-        <v>0.626053828171</v>
+        <v>0.6580349396039999</v>
       </c>
       <c r="G20" t="n">
-        <v>3.104905129627</v>
+        <v>3.106009418644</v>
       </c>
       <c r="H20" t="n">
-        <v>14.103326091313</v>
+        <v>14.958435238699</v>
       </c>
     </row>
     <row r="21">
@@ -13191,25 +13191,25 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2.62130238635</v>
+        <v>2.73851303465</v>
       </c>
       <c r="C21" t="n">
-        <v>3.490150480608</v>
+        <v>3.678294365984</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.298312575794</v>
+        <v>0.312501457719</v>
       </c>
       <c r="F21" t="n">
-        <v>0.392738456953</v>
+        <v>0.400380214623</v>
       </c>
       <c r="G21" t="n">
-        <v>1.283364939245</v>
+        <v>1.285402719861</v>
       </c>
       <c r="H21" t="n">
-        <v>1.515734508617</v>
+        <v>1.680009973781</v>
       </c>
     </row>
     <row r="22">
@@ -13219,25 +13219,25 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>6.902424242379</v>
+        <v>9.060058627965001</v>
       </c>
       <c r="C22" t="n">
-        <v>16.044331329042</v>
+        <v>16.711108458279</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>6.886191772777</v>
       </c>
       <c r="E22" t="n">
-        <v>1.009078030862</v>
+        <v>1.033217587296</v>
       </c>
       <c r="F22" t="n">
-        <v>1.301828963912</v>
+        <v>1.324363806525</v>
       </c>
       <c r="G22" t="n">
         <v>4.764456462688</v>
       </c>
       <c r="H22" t="n">
-        <v>8.96896787158</v>
+        <v>9.58907060177</v>
       </c>
     </row>
     <row r="23">
@@ -13247,25 +13247,25 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>30.324474241809</v>
+        <v>32.091794037805</v>
       </c>
       <c r="C23" t="n">
-        <v>73.96443146753199</v>
+        <v>75.087426312887</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>5.821944522571</v>
       </c>
       <c r="E23" t="n">
-        <v>9.667614148404001</v>
+        <v>9.721309019601</v>
       </c>
       <c r="F23" t="n">
-        <v>14.984920412779</v>
+        <v>15.025141649732</v>
       </c>
       <c r="G23" t="n">
-        <v>45.641090097524</v>
+        <v>45.644691619635</v>
       </c>
       <c r="H23" t="n">
-        <v>3.670806808826</v>
+        <v>4.69628402392</v>
       </c>
     </row>
     <row r="24">
@@ -13275,25 +13275,25 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>31.277000151267</v>
+        <v>33.521998891986</v>
       </c>
       <c r="C24" t="n">
-        <v>63.958239921185</v>
+        <v>64.779632958417</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>8.298155972867001</v>
       </c>
       <c r="E24" t="n">
-        <v>7.892034938911</v>
+        <v>7.9334053178</v>
       </c>
       <c r="F24" t="n">
-        <v>12.030566801837</v>
+        <v>12.060350452148</v>
       </c>
       <c r="G24" t="n">
-        <v>36.95395964004</v>
+        <v>36.957172938062</v>
       </c>
       <c r="H24" t="n">
-        <v>7.081678540396</v>
+        <v>7.828704250407</v>
       </c>
     </row>
     <row r="25">
@@ -13303,25 +13303,25 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>28.926922157342</v>
+        <v>31.28804377101</v>
       </c>
       <c r="C25" t="n">
-        <v>30.234928060939</v>
+        <v>36.364434529733</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>3.677841812699</v>
       </c>
       <c r="E25" t="n">
-        <v>2.750149011376</v>
+        <v>3.043912627874</v>
       </c>
       <c r="F25" t="n">
-        <v>3.843353725385</v>
+        <v>4.063007980608</v>
       </c>
       <c r="G25" t="n">
-        <v>12.410429637981</v>
+        <v>12.430277265959</v>
       </c>
       <c r="H25" t="n">
-        <v>11.230995686197</v>
+        <v>16.827236655292</v>
       </c>
     </row>
     <row r="26">
@@ -13331,13 +13331,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>33.860706510419</v>
+        <v>35.648243848502</v>
       </c>
       <c r="C26" t="n">
         <v>7.922132740869</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>7.506906054268</v>
       </c>
       <c r="E26" t="n">
         <v>0.852841397914</v>
@@ -13359,25 +13359,25 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2.771870804236</v>
+        <v>2.867210129541</v>
       </c>
       <c r="C27" t="n">
-        <v>15.468837872322</v>
+        <v>15.945534498847</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0.872174254897</v>
+        <v>0.958464295552</v>
       </c>
       <c r="F27" t="n">
-        <v>1.09807102417</v>
+        <v>1.12618817388</v>
       </c>
       <c r="G27" t="n">
-        <v>4.186092734245</v>
+        <v>4.205160599306</v>
       </c>
       <c r="H27" t="n">
-        <v>9.31249985901</v>
+        <v>9.655721430108001</v>
       </c>
     </row>
     <row r="28">
@@ -13471,25 +13471,25 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.77568652195</v>
+        <v>2.275003206989</v>
       </c>
       <c r="C31" t="n">
-        <v>4.566925211435</v>
+        <v>4.744709609234</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>6.063359893513</v>
       </c>
       <c r="E31" t="n">
-        <v>0.228201014274</v>
+        <v>0.235022830419</v>
       </c>
       <c r="F31" t="n">
-        <v>0.211554672035</v>
+        <v>0.217630227123</v>
       </c>
       <c r="G31" t="n">
-        <v>0.868795370635</v>
+        <v>0.868901832608</v>
       </c>
       <c r="H31" t="n">
-        <v>3.25837415449</v>
+        <v>3.423154719085</v>
       </c>
     </row>
     <row r="32">
@@ -13499,25 +13499,25 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2.626656113261</v>
+        <v>2.626663785196</v>
       </c>
       <c r="C32" t="n">
-        <v>1.674962562659</v>
+        <v>1.675000922335</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>0.071658536945</v>
+        <v>0.071665480686</v>
       </c>
       <c r="F32" t="n">
-        <v>0.037523594243</v>
+        <v>0.037525856824</v>
       </c>
       <c r="G32" t="n">
-        <v>0.198625550177</v>
+        <v>0.198627084564</v>
       </c>
       <c r="H32" t="n">
-        <v>1.367154881295</v>
+        <v>1.367182500262</v>
       </c>
     </row>
     <row r="33">
@@ -13555,25 +13555,25 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.174065238514</v>
+        <v>1.771125019121</v>
       </c>
       <c r="C34" t="n">
-        <v>0.431011701172</v>
+        <v>0.491036267144</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>5.493589776109</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.005349578847</v>
+        <v>-0.003176489318</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.042653850058</v>
+        <v>-0.040625219969</v>
       </c>
       <c r="G34" t="n">
         <v>-0.104727925172</v>
       </c>
       <c r="H34" t="n">
-        <v>0.58374305525</v>
+        <v>0.639565901603</v>
       </c>
     </row>
     <row r="35">
@@ -13583,25 +13583,25 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.490881802449</v>
+        <v>0.615513330622</v>
       </c>
       <c r="C35" t="n">
-        <v>0.717429381483</v>
+        <v>0.920630163912</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>0.301418625235</v>
       </c>
       <c r="E35" t="n">
-        <v>0.052508701027</v>
+        <v>0.059865247225</v>
       </c>
       <c r="F35" t="n">
-        <v>0.058812330384</v>
+        <v>0.065679838957</v>
       </c>
       <c r="G35" t="n">
         <v>0.195788610014</v>
       </c>
       <c r="H35" t="n">
-        <v>0.410319740057</v>
+        <v>0.599296467717</v>
       </c>
     </row>
   </sheetData>
@@ -14685,25 +14685,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>38.074224921152</v>
+        <v>61.903870885585</v>
       </c>
       <c r="C2" t="n">
-        <v>39.064550349542</v>
+        <v>42.605781615472</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>91.25258076503501</v>
       </c>
       <c r="E2" t="n">
-        <v>6.661121858274</v>
+        <v>6.789326243581</v>
       </c>
       <c r="F2" t="n">
-        <v>5.620737949281</v>
+        <v>5.74041975259</v>
       </c>
       <c r="G2" t="n">
         <v>8.261825862256</v>
       </c>
       <c r="H2" t="n">
-        <v>18.520864679731</v>
+        <v>21.814209757046</v>
       </c>
     </row>
     <row r="3">
@@ -14713,25 +14713,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10.541061879482</v>
+        <v>11.169190318332</v>
       </c>
       <c r="C3" t="n">
-        <v>19.878316549725</v>
+        <v>20.310452643837</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1.916625881393</v>
       </c>
       <c r="E3" t="n">
-        <v>4.778541343361</v>
+        <v>4.798937537864</v>
       </c>
       <c r="F3" t="n">
-        <v>3.618777931538</v>
+        <v>3.634209081584</v>
       </c>
       <c r="G3" t="n">
-        <v>3.186460255261</v>
+        <v>3.187772683016</v>
       </c>
       <c r="H3" t="n">
-        <v>8.294537019565</v>
+        <v>8.689533341372</v>
       </c>
     </row>
     <row r="4">
@@ -14741,25 +14741,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>23.880593665894</v>
+        <v>30.004575470125</v>
       </c>
       <c r="C4" t="n">
-        <v>33.603236068177</v>
+        <v>36.091123525941</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>20.503099276167</v>
       </c>
       <c r="E4" t="n">
-        <v>5.70029704994</v>
+        <v>5.795758752452</v>
       </c>
       <c r="F4" t="n">
-        <v>4.990086541886</v>
+        <v>5.075106620442</v>
       </c>
       <c r="G4" t="n">
-        <v>7.818154874814</v>
+        <v>7.819644206349</v>
       </c>
       <c r="H4" t="n">
-        <v>15.094697601537</v>
+        <v>17.400613946699</v>
       </c>
     </row>
     <row r="5">
@@ -14769,25 +14769,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7.755294115269</v>
+        <v>8.003822772179999</v>
       </c>
       <c r="C5" t="n">
-        <v>17.268067359261</v>
+        <v>17.774890718204</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.002901343633</v>
       </c>
       <c r="E5" t="n">
-        <v>4.609139243975</v>
+        <v>4.636516067349</v>
       </c>
       <c r="F5" t="n">
-        <v>3.438622785908</v>
+        <v>3.457321941384</v>
       </c>
       <c r="G5" t="n">
-        <v>2.24284574314</v>
+        <v>2.245339471075</v>
       </c>
       <c r="H5" t="n">
-        <v>6.977459586237</v>
+        <v>7.435713238396</v>
       </c>
     </row>
     <row r="6">
@@ -14797,25 +14797,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>226.654883097924</v>
+        <v>297.50503499857</v>
       </c>
       <c r="C6" t="n">
-        <v>241.870969550293</v>
+        <v>255.869631186432</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>261.482648963137</v>
       </c>
       <c r="E6" t="n">
-        <v>42.987521374056</v>
+        <v>43.782861376658</v>
       </c>
       <c r="F6" t="n">
-        <v>36.988877398015</v>
+        <v>37.512170076787</v>
       </c>
       <c r="G6" t="n">
-        <v>54.831317411162</v>
+        <v>54.911017732772</v>
       </c>
       <c r="H6" t="n">
-        <v>107.063253367061</v>
+        <v>119.663582000215</v>
       </c>
     </row>
     <row r="7">
@@ -14825,25 +14825,25 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6.989702771929</v>
+        <v>7.008998436843</v>
       </c>
       <c r="C7" t="n">
-        <v>18.726926660049</v>
+        <v>18.785060136812</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>4.94455310752</v>
+        <v>4.94665773331</v>
       </c>
       <c r="F7" t="n">
-        <v>3.601368421146</v>
+        <v>3.603333138728</v>
       </c>
       <c r="G7" t="n">
         <v>2.052983876997</v>
       </c>
       <c r="H7" t="n">
-        <v>8.128021254387001</v>
+        <v>8.182085387776</v>
       </c>
     </row>
     <row r="8">
@@ -14853,25 +14853,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>13.073339097183</v>
+        <v>13.283654392257</v>
       </c>
       <c r="C8" t="n">
-        <v>19.595525907983</v>
+        <v>20.109092386825</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.311133572002</v>
       </c>
       <c r="E8" t="n">
-        <v>2.622996300455</v>
+        <v>2.642664310543</v>
       </c>
       <c r="F8" t="n">
-        <v>1.747880561855</v>
+        <v>1.76542439803</v>
       </c>
       <c r="G8" t="n">
-        <v>1.910132276089</v>
+        <v>1.910429262617</v>
       </c>
       <c r="H8" t="n">
-        <v>13.314516769585</v>
+        <v>13.790574415636</v>
       </c>
     </row>
     <row r="9">
@@ -14881,25 +14881,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>85.33632794001601</v>
+        <v>99.749990168997</v>
       </c>
       <c r="C9" t="n">
-        <v>129.621237997239</v>
+        <v>136.178480435893</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>51.155460067742</v>
       </c>
       <c r="E9" t="n">
-        <v>24.92588927246</v>
+        <v>25.251509324135</v>
       </c>
       <c r="F9" t="n">
-        <v>18.957911352594</v>
+        <v>19.194868976429</v>
       </c>
       <c r="G9" t="n">
-        <v>19.636521087386</v>
+        <v>19.660890664987</v>
       </c>
       <c r="H9" t="n">
-        <v>66.100916284799</v>
+        <v>72.071211470343</v>
       </c>
     </row>
     <row r="10">
@@ -14909,25 +14909,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>116.452946762147</v>
+        <v>146.874493176789</v>
       </c>
       <c r="C10" t="n">
-        <v>135.300213129411</v>
+        <v>146.180372944656</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>110.843643038932</v>
       </c>
       <c r="E10" t="n">
-        <v>31.575176103669</v>
+        <v>32.046273520758</v>
       </c>
       <c r="F10" t="n">
-        <v>25.258032270896</v>
+        <v>25.639172268579</v>
       </c>
       <c r="G10" t="n">
-        <v>25.527270834072</v>
+        <v>25.548594652355</v>
       </c>
       <c r="H10" t="n">
-        <v>52.939733920775</v>
+        <v>62.946332502965</v>
       </c>
     </row>
     <row r="11">
@@ -14937,25 +14937,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3.911138237069</v>
+        <v>4.877560272643</v>
       </c>
       <c r="C11" t="n">
-        <v>8.051334131775</v>
+        <v>9.047951425955</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>2.393117889847</v>
       </c>
       <c r="E11" t="n">
-        <v>1.605619353348</v>
+        <v>1.642433989497</v>
       </c>
       <c r="F11" t="n">
-        <v>1.165020712888</v>
+        <v>1.198830672859</v>
       </c>
       <c r="G11" t="n">
-        <v>0.948549639453</v>
+        <v>0.9487523184</v>
       </c>
       <c r="H11" t="n">
-        <v>4.332144426085</v>
+        <v>5.257934445199</v>
       </c>
     </row>
     <row r="12">
@@ -14965,25 +14965,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>118.088329723745</v>
+        <v>136.032029253776</v>
       </c>
       <c r="C12" t="n">
-        <v>111.362838691183</v>
+        <v>121.373769844268</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>61.473070552521</v>
       </c>
       <c r="E12" t="n">
-        <v>17.211340861443</v>
+        <v>17.81246623503</v>
       </c>
       <c r="F12" t="n">
-        <v>14.279066103934</v>
+        <v>14.658917421462</v>
       </c>
       <c r="G12" t="n">
-        <v>21.786960512828</v>
+        <v>21.852892632922</v>
       </c>
       <c r="H12" t="n">
-        <v>58.085471212978</v>
+        <v>67.049493554854</v>
       </c>
     </row>
     <row r="13">
@@ -14993,25 +14993,25 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3.319385704562</v>
+        <v>3.345196342962</v>
       </c>
       <c r="C13" t="n">
-        <v>8.287197390684</v>
+        <v>8.365883264024999</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>2.326929734166</v>
+        <v>2.329778425276</v>
       </c>
       <c r="F13" t="n">
-        <v>1.711179518389</v>
+        <v>1.713838838413</v>
       </c>
       <c r="G13" t="n">
         <v>0.953959479075</v>
       </c>
       <c r="H13" t="n">
-        <v>3.295128659053</v>
+        <v>3.36830652126</v>
       </c>
     </row>
     <row r="14">
@@ -15021,25 +15021,25 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.918736023948</v>
+        <v>2.03872843949</v>
       </c>
       <c r="C14" t="n">
-        <v>2.231782381767</v>
+        <v>2.761270169336</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0.233256430585</v>
+        <v>0.252425654856</v>
       </c>
       <c r="F14" t="n">
-        <v>0.158507779303</v>
+        <v>0.176402700161</v>
       </c>
       <c r="G14" t="n">
         <v>0.247011753276</v>
       </c>
       <c r="H14" t="n">
-        <v>1.593006418603</v>
+        <v>2.085430061043</v>
       </c>
     </row>
     <row r="15">
@@ -15049,25 +15049,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>16.356289940323</v>
+        <v>24.683473908554</v>
       </c>
       <c r="C15" t="n">
-        <v>21.782809451484</v>
+        <v>23.102839254775</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>30.368723434658</v>
       </c>
       <c r="E15" t="n">
-        <v>5.434834785183</v>
+        <v>5.500722209193</v>
       </c>
       <c r="F15" t="n">
-        <v>4.161198323653</v>
+        <v>4.208958611296</v>
       </c>
       <c r="G15" t="n">
-        <v>3.304120052032</v>
+        <v>3.30911902272</v>
       </c>
       <c r="H15" t="n">
-        <v>8.882656290615</v>
+        <v>10.084039411567</v>
       </c>
     </row>
     <row r="16">
@@ -15077,25 +15077,25 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>32.61605301576</v>
+        <v>73.311326008815</v>
       </c>
       <c r="C16" t="n">
-        <v>54.775584410706</v>
+        <v>57.080695020703</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>152.766053424734</v>
       </c>
       <c r="E16" t="n">
-        <v>12.69041189071</v>
+        <v>12.782970710009</v>
       </c>
       <c r="F16" t="n">
-        <v>10.090441984788</v>
+        <v>10.169930816164</v>
       </c>
       <c r="G16" t="n">
-        <v>9.92515368924</v>
+        <v>9.927668961705001</v>
       </c>
       <c r="H16" t="n">
-        <v>22.069576845969</v>
+        <v>24.200124532825</v>
       </c>
     </row>
     <row r="17">
@@ -15105,25 +15105,25 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>27.324702183036</v>
+        <v>29.694370737225</v>
       </c>
       <c r="C17" t="n">
-        <v>28.603208784809</v>
+        <v>28.978984350772</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>9.119645263137</v>
       </c>
       <c r="E17" t="n">
-        <v>3.088139054648</v>
+        <v>3.156160699988</v>
       </c>
       <c r="F17" t="n">
-        <v>4.190987147738</v>
+        <v>4.213151638229</v>
       </c>
       <c r="G17" t="n">
-        <v>12.575656699503</v>
+        <v>12.590687722142</v>
       </c>
       <c r="H17" t="n">
-        <v>8.748425882919999</v>
+        <v>9.018984290413</v>
       </c>
     </row>
     <row r="18">
@@ -15133,25 +15133,25 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>56.402375498235</v>
+        <v>68.820966730164</v>
       </c>
       <c r="C18" t="n">
-        <v>113.284653229714</v>
+        <v>117.476365007782</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>41.474630778511</v>
       </c>
       <c r="E18" t="n">
-        <v>26.891325025203</v>
+        <v>27.050056281869</v>
       </c>
       <c r="F18" t="n">
-        <v>20.320144184304</v>
+        <v>20.463023586792</v>
       </c>
       <c r="G18" t="n">
-        <v>16.674092829891</v>
+        <v>16.676020085112</v>
       </c>
       <c r="H18" t="n">
-        <v>49.399091190316</v>
+        <v>53.287265054009</v>
       </c>
     </row>
     <row r="19">
@@ -15161,25 +15161,25 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>16.178392938704</v>
+        <v>20.78039371997</v>
       </c>
       <c r="C19" t="n">
-        <v>30.990625921084</v>
+        <v>33.335563571054</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>15.652892113115</v>
       </c>
       <c r="E19" t="n">
-        <v>5.68534760326</v>
+        <v>5.776758014521</v>
       </c>
       <c r="F19" t="n">
-        <v>5.172523014212</v>
+        <v>5.252907352356</v>
       </c>
       <c r="G19" t="n">
-        <v>8.460343545945999</v>
+        <v>8.462143337454</v>
       </c>
       <c r="H19" t="n">
-        <v>11.672411757667</v>
+        <v>13.843754866723</v>
       </c>
     </row>
     <row r="20">
@@ -15189,25 +15189,25 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>26.345266305531</v>
+        <v>29.098822469104</v>
       </c>
       <c r="C20" t="n">
-        <v>56.17779545521</v>
+        <v>57.10350154631</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>9.698948804879</v>
       </c>
       <c r="E20" t="n">
-        <v>11.946066160487</v>
+        <v>11.983577703751</v>
       </c>
       <c r="F20" t="n">
-        <v>8.956526555650001</v>
+        <v>8.988507667083001</v>
       </c>
       <c r="G20" t="n">
-        <v>7.621648009161</v>
+        <v>7.622752298177</v>
       </c>
       <c r="H20" t="n">
-        <v>27.653554729913</v>
+        <v>28.508663877298</v>
       </c>
     </row>
     <row r="21">
@@ -15217,25 +15217,25 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>6.969943285801</v>
+        <v>7.087153934101</v>
       </c>
       <c r="C21" t="n">
-        <v>9.334342520391001</v>
+        <v>9.522486405766999</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>2.043841371409</v>
+        <v>2.058030253334</v>
       </c>
       <c r="F21" t="n">
-        <v>1.686189522025</v>
+        <v>1.693831279695</v>
       </c>
       <c r="G21" t="n">
-        <v>1.984667984019</v>
+        <v>1.986705764635</v>
       </c>
       <c r="H21" t="n">
-        <v>3.619643642938</v>
+        <v>3.783919108103</v>
       </c>
     </row>
     <row r="22">
@@ -15245,25 +15245,25 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>13.036384106071</v>
+        <v>15.194018491657</v>
       </c>
       <c r="C22" t="n">
-        <v>16.044331329042</v>
+        <v>16.711108458279</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>6.886191772777</v>
       </c>
       <c r="E22" t="n">
-        <v>1.009078030862</v>
+        <v>1.033217587296</v>
       </c>
       <c r="F22" t="n">
-        <v>1.301828963912</v>
+        <v>1.324363806525</v>
       </c>
       <c r="G22" t="n">
         <v>4.764456462688</v>
       </c>
       <c r="H22" t="n">
-        <v>8.96896787158</v>
+        <v>9.58907060177</v>
       </c>
     </row>
     <row r="23">
@@ -15273,25 +15273,25 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>48.038412286</v>
+        <v>49.805732081996</v>
       </c>
       <c r="C23" t="n">
-        <v>93.33901930997899</v>
+        <v>94.462014155334</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>5.821944522571</v>
       </c>
       <c r="E23" t="n">
-        <v>15.45436803191</v>
+        <v>15.508062903107</v>
       </c>
       <c r="F23" t="n">
-        <v>19.272952207345</v>
+        <v>19.313173444298</v>
       </c>
       <c r="G23" t="n">
-        <v>47.966040638617</v>
+        <v>47.969642160729</v>
       </c>
       <c r="H23" t="n">
-        <v>10.645658432107</v>
+        <v>11.671135647201</v>
       </c>
     </row>
     <row r="24">
@@ -15301,25 +15301,25 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>55.001332367501</v>
+        <v>57.246331108219</v>
       </c>
       <c r="C24" t="n">
-        <v>69.452314287929</v>
+        <v>70.27370732516199</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>8.298155972867001</v>
       </c>
       <c r="E24" t="n">
-        <v>9.53299145559</v>
+        <v>9.574361834478999</v>
       </c>
       <c r="F24" t="n">
-        <v>13.246528955866</v>
+        <v>13.276312606176</v>
       </c>
       <c r="G24" t="n">
-        <v>37.613248564049</v>
+        <v>37.616461862071</v>
       </c>
       <c r="H24" t="n">
-        <v>9.059545312425</v>
+        <v>9.806571022435</v>
       </c>
     </row>
     <row r="25">
@@ -15329,25 +15329,25 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>90.23245398413</v>
+        <v>92.59357559779799</v>
       </c>
       <c r="C25" t="n">
-        <v>109.928853088004</v>
+        <v>116.058359556798</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>3.677841812699</v>
       </c>
       <c r="E25" t="n">
-        <v>26.552933044381</v>
+        <v>26.846696660878</v>
       </c>
       <c r="F25" t="n">
-        <v>21.481410706454</v>
+        <v>21.701064961678</v>
       </c>
       <c r="G25" t="n">
-        <v>21.973700641229</v>
+        <v>21.993548269207</v>
       </c>
       <c r="H25" t="n">
-        <v>39.92080869594</v>
+        <v>45.517049665036</v>
       </c>
     </row>
     <row r="26">
@@ -15357,13 +15357,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>49.955517179325</v>
+        <v>51.743054517408</v>
       </c>
       <c r="C26" t="n">
         <v>22.262406787962</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>7.506906054268</v>
       </c>
       <c r="E26" t="n">
         <v>5.135958912846</v>
@@ -15385,25 +15385,25 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>16.825729752964</v>
+        <v>16.921069078269</v>
       </c>
       <c r="C27" t="n">
-        <v>29.419317596056</v>
+        <v>29.896014222581</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>5.038868967299</v>
+        <v>5.125159007954</v>
       </c>
       <c r="F27" t="n">
-        <v>4.185625768109</v>
+        <v>4.21374291782</v>
       </c>
       <c r="G27" t="n">
-        <v>5.860150301093</v>
+        <v>5.879218166154</v>
       </c>
       <c r="H27" t="n">
-        <v>14.334672559555</v>
+        <v>14.677894130653</v>
       </c>
     </row>
     <row r="28">
@@ -15497,25 +15497,25 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>8.220824091175</v>
+        <v>9.720140776215</v>
       </c>
       <c r="C31" t="n">
-        <v>14.991192137555</v>
+        <v>15.168976535354</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>6.063359893513</v>
       </c>
       <c r="E31" t="n">
-        <v>3.341695226795</v>
+        <v>3.348517042939</v>
       </c>
       <c r="F31" t="n">
-        <v>2.518679261097</v>
+        <v>2.524754816185</v>
       </c>
       <c r="G31" t="n">
-        <v>2.119707401769</v>
+        <v>2.119813863743</v>
       </c>
       <c r="H31" t="n">
-        <v>7.011110247894</v>
+        <v>7.175890812488</v>
       </c>
     </row>
     <row r="32">
@@ -15525,25 +15525,25 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>4.209077428929</v>
+        <v>4.209085100864</v>
       </c>
       <c r="C32" t="n">
-        <v>4.234586411599</v>
+        <v>4.234624771274</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>0.836160644995</v>
+        <v>0.836167588737</v>
       </c>
       <c r="F32" t="n">
-        <v>0.60402588764</v>
+        <v>0.604028150221</v>
       </c>
       <c r="G32" t="n">
-        <v>0.50578041205</v>
+        <v>0.505781946437</v>
       </c>
       <c r="H32" t="n">
-        <v>2.288619466914</v>
+        <v>2.28864708588</v>
       </c>
     </row>
     <row r="33">
@@ -15581,25 +15581,25 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1.627421316817</v>
+        <v>3.224481097424</v>
       </c>
       <c r="C34" t="n">
-        <v>6.526421142651</v>
+        <v>6.586445708622</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>5.493589776109</v>
       </c>
       <c r="E34" t="n">
-        <v>1.81521220775</v>
+        <v>1.817385297279</v>
       </c>
       <c r="F34" t="n">
-        <v>1.306397272913</v>
+        <v>1.308425903002</v>
       </c>
       <c r="G34" t="n">
         <v>0.626721207806</v>
       </c>
       <c r="H34" t="n">
-        <v>2.778090454182</v>
+        <v>2.833913300536</v>
       </c>
     </row>
     <row r="35">
@@ -15609,25 +15609,25 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>2.308884081094</v>
+        <v>2.433515609268</v>
       </c>
       <c r="C35" t="n">
-        <v>3.027672653441</v>
+        <v>3.23087343587</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>0.301418625235</v>
       </c>
       <c r="E35" t="n">
-        <v>0.742526436349</v>
+        <v>0.749882982547</v>
       </c>
       <c r="F35" t="n">
-        <v>0.57012109648</v>
+        <v>0.576988605052</v>
       </c>
       <c r="G35" t="n">
         <v>0.473017802649</v>
       </c>
       <c r="H35" t="n">
-        <v>1.242007317962</v>
+        <v>1.430984045622</v>
       </c>
     </row>
   </sheetData>
@@ -15726,25 +15726,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.006562138778</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.032810693892</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.005939282874</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.00193528366</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.001312427756</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>0.023623699602</v>
       </c>
     </row>
     <row r="4">
@@ -15754,25 +15754,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.007446657675</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.037233288376</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.006739846244</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.002196142966</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.001489331535</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>0.026807967631</v>
       </c>
     </row>
     <row r="5">
@@ -15782,25 +15782,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.012468639675</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.062343198373</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.011285158784</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.003677208825</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.002493727935</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>0.044887102828</v>
       </c>
     </row>
     <row r="6">
@@ -15810,25 +15810,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>0.398501608053</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1.992508040266</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.360677190132</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.117524739531</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.07970032161100001</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>1.434605788991</v>
       </c>
     </row>
     <row r="7">
@@ -15866,25 +15866,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.00148493264</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>0.0074246632</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.001343987882</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.000437931286</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>0.000296986528</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>0.005345757504</v>
       </c>
     </row>
     <row r="9">
@@ -15894,25 +15894,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>0.121847888004</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.60923944002</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.110282500699</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.035934964905</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>0.024369577601</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>0.438652396815</v>
       </c>
     </row>
     <row r="10">
@@ -15922,25 +15922,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>0.106619091417</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.533095457084</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.09649916971399999</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.031443739987</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.021323818283</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.383828729101</v>
       </c>
     </row>
     <row r="11">
@@ -15950,25 +15950,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>0.001013394737</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.005066973686</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>0.000917206754</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.000298866931</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.000202678947</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>0.003648221054</v>
       </c>
     </row>
     <row r="12">
@@ -15978,25 +15978,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>0.32966060047</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>1.648303002351</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.298370336962</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>0.097222383602</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.065932120094</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>1.186778161693</v>
       </c>
     </row>
     <row r="13">
@@ -16062,25 +16062,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>0.024994853437</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>0.124974267186</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>0.02262242692</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>0.007371397205</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>0.004998970687</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>0.089981472374</v>
       </c>
     </row>
     <row r="16">
@@ -16090,25 +16090,25 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>0.012576362324</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>0.062881811619</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>0.011382656766</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>0.003708978023</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>0.002515272465</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>0.045274904366</v>
       </c>
     </row>
     <row r="17">
@@ -16118,25 +16118,25 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>0.075155113193</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>0.375775565963</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>0.06802164534000001</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>0.022164490491</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>0.015031022639</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>0.270558407493</v>
       </c>
     </row>
     <row r="18">
@@ -16146,25 +16146,25 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>0.009636276104999999</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>0.048181380527</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>0.008721633536000001</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>0.00284189779</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>0.001927255221</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>0.034690593979</v>
       </c>
     </row>
     <row r="19">
@@ -16174,25 +16174,25 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>0.008998957538000001</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>0.044994787692</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>0.008144807081000001</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>0.002653941965</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>0.001799791508</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>0.032396247138</v>
       </c>
     </row>
     <row r="20">
@@ -16202,25 +16202,25 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>0.005521445083</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>0.027607225414</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>0.004997368286</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>0.001628365814</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>0.001104289017</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>0.019877202298</v>
       </c>
     </row>
     <row r="21">
@@ -16230,25 +16230,25 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>0.010188903081</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>0.050944515405</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>0.009221807037999999</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>0.003004876659</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>0.002037780616</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>0.036680051092</v>
       </c>
     </row>
     <row r="22">
@@ -16286,25 +16286,25 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>0.018007610559</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>0.090038052794</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>0.016298389382</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>0.005310743289</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>0.003601522112</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>0.06482739801200001</v>
       </c>
     </row>
     <row r="24">
@@ -16314,25 +16314,25 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>0.01606649011</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>0.08033245054800001</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>0.014541513487</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>0.004738274645</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>0.003213298022</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>0.057839364395</v>
       </c>
     </row>
     <row r="25">
@@ -16342,25 +16342,25 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>0.099238139889</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>0.496190699443</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>0.089818793013</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>0.029266974854</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>0.019847627978</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>0.357257303599</v>
       </c>
     </row>
     <row r="26">
@@ -16398,25 +16398,25 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>0.095339325305</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>0.476696626525</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>0.086290040655</v>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
+        <v>0.028117149711</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>0.019067865061</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>0.343221571098</v>
       </c>
     </row>
     <row r="28">
@@ -16510,25 +16510,25 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>0.000532309866</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>0.00266154933</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>0.000481784823</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>0.000156987016</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>0.000106461973</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>0.001916315518</v>
       </c>
     </row>
     <row r="32">
@@ -16538,25 +16538,25 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>7.671934999999999e-06</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>3.8359675e-05</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>6.943741e-06</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>2.262581e-06</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>1.534387e-06</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>2.7618966e-05</v>
       </c>
     </row>
     <row r="33">
@@ -19750,13 +19750,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1.433399921234</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>4.945777152718</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -19778,13 +19778,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.555482243253</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1.916625881393</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -19806,13 +19806,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.341443044515</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1.178108902825</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -19834,13 +19834,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.000382590765</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.001320084255</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -19862,13 +19862,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>4.446944735941</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>15.343657655208</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -19918,13 +19918,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.090173662062</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.311133572002</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -19946,13 +19946,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>0.720391388186</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>2.485625411252</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -19974,13 +19974,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>1.296908259669</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>4.474828793294</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -20002,13 +20002,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>0.567340150405</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1.957540189674</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -20030,13 +20030,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>0.519135700764</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>1.791216428832</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -20114,13 +20114,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>0.515727142588</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>1.779455601375</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -20142,13 +20142,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>3.113907311378</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>10.744169445076</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -20170,13 +20170,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>0.689200223203</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>2.378003979958</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -20198,13 +20198,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>3.537800793519</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>12.206763846052</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -20254,13 +20254,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>1.296201807914</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>4.472391264941</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -20310,13 +20310,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>0.686852663801</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>2.369904003472</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -20394,13 +20394,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>0.540158031425</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>1.863751498172</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -20562,13 +20562,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>0.128138813869</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>0.442127844869</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -20646,13 +20646,13 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>1.344297238115</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>4.638338867083</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -20674,13 +20674,13 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0</v>
+        <v>0.087334237759</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>0.301336473763</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -20763,13 +20763,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.008256163083</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.034672417362</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -20819,13 +20819,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.000719347131</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.003020955826</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -20847,13 +20847,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.000376527981</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.001581259378</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -20875,13 +20875,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1.696470907868</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>7.124465295265</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -20959,13 +20959,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>0.001222239617</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>0.005132893052</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -20987,13 +20987,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>0.019648408762</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.082515064471</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -21015,13 +21015,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>1.994361e-06</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>8.375478e-06</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -21127,13 +21127,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>0.000154468194</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>0.000648701539</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -21155,13 +21155,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>0.720384094998</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>3.025310637673</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -21267,13 +21267,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>1.5150343e-05</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>6.3625079e-05</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -21407,13 +21407,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>0.000247170631</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>0.001038012837</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -21435,13 +21435,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>1.083406038085</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>4.549850329423</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -21575,13 +21575,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>0.249121017317</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>1.046203641903</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -21776,13 +21776,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>10.655732703445</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>44.749601946734</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -21832,13 +21832,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.865289707205</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>3.633853348586</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -21888,13 +21888,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>19.818637978567</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>83.229955682031</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -21972,13 +21972,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>3.18104219616</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>13.359041186148</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -22000,13 +22000,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>10.090444722874</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>42.375629849286</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -22056,13 +22056,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>3.9648369516</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>16.650649965202</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -22140,13 +22140,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>2.323991438779</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>9.759787966468</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -22168,13 +22168,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>10.058909307733</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>42.243194350568</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -22196,13 +22196,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>0.802656608897</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>3.37082064159</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -22224,13 +22224,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>1.900560890159</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>7.981557503092</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -22252,13 +22252,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>1.189987413239</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>4.997447340889</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -22336,13 +22336,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>0.143994170322</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>0.604715037802</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -22364,13 +22364,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>0.713191416181</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>2.995104407565</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -22392,13 +22392,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>0.8312925729840001</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>3.491079663652</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -22588,13 +22588,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>0.682208324344</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>2.86498843475</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>

</xml_diff>